<commit_message>
Ajustes nos documentos de teste
Adicionado passos nos casos de teste relacionado ao cadastro de projeto
e usuário já cadastrados.
</commit_message>
<xml_diff>
--- a/trunk/doc/testes/CT - Manter Projeto.xlsx
+++ b/trunk/doc/testes/CT - Manter Projeto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="570" windowWidth="23655" windowHeight="9405"/>
+    <workbookView xWindow="150" yWindow="570" windowWidth="20730" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Scrumming</t>
   </si>
@@ -152,6 +152,23 @@
   </si>
   <si>
     <t>O projeto não deverá ter sua situação alterada exibindo a mensagem de que existe alguma dependência a ser resolvida para que a alteração da situação seja executada.</t>
+  </si>
+  <si>
+    <t>02.00 - 09/04/2014</t>
+  </si>
+  <si>
+    <t>Efetuar o cadastro de projeto sem sucesso. Projeto já existe.
+Passo #1 e #2 executados com sucesso;
+Deve existir Projeto cadastrado.</t>
+  </si>
+  <si>
+    <t>1- Executar o passo #1 acessando a tela de criação de projetos.
+2- Preencher os campos obrigatórios com informações de projetos já cadastrados.
+3- Acionar a opção de Salvar.</t>
+  </si>
+  <si>
+    <t>O sistema não deverá permitir salvar o novo projeto informando mensagem de que projeto já está cadastrado.
+"Já existe Projeto cadastrado com o nome informado."</t>
   </si>
 </sst>
 </file>
@@ -594,8 +611,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -742,11 +763,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.75">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:4" ht="63.75">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="4"/>

</xml_diff>